<commit_message>
Prepared files for tensorboard visualization (TL)
</commit_message>
<xml_diff>
--- a/log/tripletloss/accuracy_without_5.xlsx
+++ b/log/tripletloss/accuracy_without_5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\humbe\Documents\TU_Dortmund\3_WS_2019_2020\Computer Vision Deep Learning\CVDL-Parametrizable-Classification\log\tripletloss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C11A54-49CC-4EAE-ACCE-5455B27C734B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE396504-3C94-49D5-A1EB-1C7EBC04122B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3204" yWindow="3204" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -59,7 +66,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -68,6 +75,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -375,7 +385,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:K11"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -435,7 +445,7 @@
       <c r="F2" s="2">
         <v>0.99889316836023356</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="4">
         <v>0.99728415697091222</v>
       </c>
       <c r="H2" s="2">
@@ -470,7 +480,7 @@
       <c r="F3" s="2">
         <v>0.9988314123550277</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="4">
         <v>0.991457787754084</v>
       </c>
       <c r="H3" s="2">
@@ -505,7 +515,7 @@
       <c r="F4" s="2">
         <v>0.9995600206048777</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="4">
         <v>0.99845093896176984</v>
       </c>
       <c r="H4" s="2">
@@ -540,7 +550,7 @@
       <c r="F5" s="2">
         <v>0.99997070201014515</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="4">
         <v>0.71542314456090472</v>
       </c>
       <c r="H5" s="2">
@@ -575,7 +585,7 @@
       <c r="F6" s="2">
         <v>0.94958491916299403</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="4">
         <v>0.99779422953055297</v>
       </c>
       <c r="H6" s="2">
@@ -610,19 +620,19 @@
       <c r="F7" s="3">
         <v>0</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="4">
         <v>0.87294905730092098</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="4">
         <v>0.95300737550824632</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="4">
         <v>0.9954090291643034</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="4">
         <v>0.9460345143798381</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="4">
         <v>0.94390109204924022</v>
       </c>
     </row>
@@ -768,5 +778,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>